<commit_message>
20% opt rank angle
</commit_message>
<xml_diff>
--- a/mnist_rankfiltering_new.xlsx
+++ b/mnist_rankfiltering_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shukl\Documents\GitHub\Mnist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBDBD96-E0F3-4A89-8027-BF05215EA74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D90C3DF-F584-4C89-8EBA-B99C465C43D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="13" xr2:uid="{99AABAAA-7628-4418-980C-C3481A48FE43}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="11" xr2:uid="{99AABAAA-7628-4418-980C-C3481A48FE43}"/>
   </bookViews>
   <sheets>
     <sheet name="ace85svm" sheetId="5" state="hidden" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Sheet2" sheetId="15" state="hidden" r:id="rId9"/>
     <sheet name="Sheet3" sheetId="16" r:id="rId10"/>
     <sheet name="dbscanclust_l1pca" sheetId="17" state="hidden" r:id="rId11"/>
-    <sheet name="comparision" sheetId="18" r:id="rId12"/>
+    <sheet name="0%" sheetId="18" r:id="rId12"/>
     <sheet name="20%contamination" sheetId="19" r:id="rId13"/>
     <sheet name="30%Contamination" sheetId="20" r:id="rId14"/>
     <sheet name="ace recur eps evm 75 percentile" sheetId="13" state="hidden" r:id="rId15"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="80">
   <si>
     <t>---------split 1 --------------------</t>
   </si>
@@ -444,13 +444,22 @@
     <t>Raw</t>
   </si>
   <si>
-    <t xml:space="preserve">diff </t>
-  </si>
-  <si>
     <t>opt</t>
   </si>
   <si>
     <t>knee opt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> l1 knee error</t>
+  </si>
+  <si>
+    <t>l1 20% excision</t>
+  </si>
+  <si>
+    <t>l1 Raw</t>
+  </si>
+  <si>
+    <t>knee optrank angle</t>
   </si>
 </sst>
 </file>
@@ -640,7 +649,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1043,11 +1052,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1305,8 +1353,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="9" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1382,23 +1428,50 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1424,12 +1497,6 @@
     <xf numFmtId="2" fontId="0" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="5" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1442,39 +1509,6 @@
     <xf numFmtId="2" fontId="5" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1486,6 +1520,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1820,10 +1866,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -2571,26 +2617,26 @@
     <row r="2" spans="2:12" ht="15" thickBot="1">
       <c r="B2" s="50"/>
       <c r="C2" s="50"/>
-      <c r="D2" s="135" t="s">
+      <c r="D2" s="133" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="136"/>
+      <c r="E2" s="134"/>
       <c r="F2" s="51"/>
-      <c r="J2" s="135" t="s">
+      <c r="J2" s="133" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="136"/>
+      <c r="K2" s="134"/>
     </row>
     <row r="3" spans="2:12" ht="14.55" customHeight="1">
-      <c r="D3" s="137" t="s">
+      <c r="D3" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="138"/>
+      <c r="E3" s="136"/>
       <c r="F3" s="52"/>
-      <c r="J3" s="137" t="s">
+      <c r="J3" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="138"/>
+      <c r="K3" s="136"/>
     </row>
     <row r="4" spans="2:12" ht="15" thickBot="1">
       <c r="D4" s="53" t="s">
@@ -2608,7 +2654,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="14.55" customHeight="1">
-      <c r="B5" s="131" t="b">
+      <c r="B5" s="129" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="57" t="s">
@@ -2622,10 +2668,10 @@
         <f>D14</f>
         <v>51.2</v>
       </c>
-      <c r="F5" s="133" t="s">
+      <c r="F5" s="131" t="s">
         <v>61</v>
       </c>
-      <c r="H5" s="131" t="b">
+      <c r="H5" s="129" t="b">
         <v>1</v>
       </c>
       <c r="I5" s="57" t="s">
@@ -2639,12 +2685,12 @@
         <f>D20</f>
         <v>51.2</v>
       </c>
-      <c r="L5" s="133" t="s">
+      <c r="L5" s="131" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:12" ht="15" thickBot="1">
-      <c r="B6" s="132"/>
+      <c r="B6" s="130"/>
       <c r="C6" s="60" t="s">
         <v>49</v>
       </c>
@@ -2656,8 +2702,8 @@
         <f>D15</f>
         <v>1838.4</v>
       </c>
-      <c r="F6" s="134"/>
-      <c r="H6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="H6" s="130"/>
       <c r="I6" s="60" t="s">
         <v>49</v>
       </c>
@@ -2669,7 +2715,7 @@
         <f>D21</f>
         <v>1775.4</v>
       </c>
-      <c r="L6" s="134"/>
+      <c r="L6" s="132"/>
     </row>
     <row r="7" spans="2:12" ht="28.8">
       <c r="D7" s="61" t="s">
@@ -2966,30 +3012,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1">
-      <c r="B1" s="145" t="s">
+      <c r="B1" s="143" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="146"/>
-      <c r="D1" s="147"/>
-      <c r="G1" s="145" t="s">
+      <c r="C1" s="144"/>
+      <c r="D1" s="145"/>
+      <c r="G1" s="143" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="146"/>
-      <c r="I1" s="147"/>
+      <c r="H1" s="144"/>
+      <c r="I1" s="145"/>
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1"/>
     <row r="3" spans="1:14" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="76"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="142"/>
+      <c r="D3" s="140"/>
       <c r="E3" s="84"/>
-      <c r="H3" s="143" t="s">
+      <c r="H3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="144"/>
+      <c r="I3" s="142"/>
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1">
       <c r="A4" s="76"/>
@@ -3009,7 +3055,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="139" t="b">
+      <c r="A5" s="137" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="77" t="s">
@@ -3032,7 +3078,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15" thickBot="1">
-      <c r="A6" s="140"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="78" t="s">
         <v>69</v>
       </c>
@@ -3125,10 +3171,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5098F06-A16F-4ADA-89BF-F72428932D91}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3138,38 +3184,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1">
-      <c r="C1" s="170" t="s">
+      <c r="C1" s="158" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="159"/>
+      <c r="E1" s="158" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="159"/>
+      <c r="G1" s="158" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="159"/>
+      <c r="I1" s="158" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="159"/>
+      <c r="K1" s="158" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="159"/>
+      <c r="N1" s="161" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="171"/>
-      <c r="E1" s="170" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="171"/>
-      <c r="G1" s="170" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="171"/>
-      <c r="I1" s="170" t="s">
+      <c r="O1" s="162"/>
+      <c r="P1" s="161" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="171"/>
-      <c r="K1" s="170" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" s="171"/>
-      <c r="N1" s="154" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" s="155"/>
-      <c r="P1" s="154" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="155"/>
-      <c r="R1" s="154" t="s">
-        <v>75</v>
-      </c>
-      <c r="S1" s="155"/>
+      <c r="Q1" s="162"/>
+      <c r="R1" s="161" t="s">
+        <v>74</v>
+      </c>
+      <c r="S1" s="162"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1">
       <c r="N2" s="113"/>
@@ -3182,38 +3228,38 @@
     <row r="3" spans="1:19" ht="15" customHeight="1" thickBot="1">
       <c r="A3" s="76"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="141" t="s">
+      <c r="D3" s="140"/>
+      <c r="E3" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="142"/>
-      <c r="G3" s="143" t="s">
+      <c r="F3" s="140"/>
+      <c r="G3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="144"/>
-      <c r="I3" s="143" t="s">
+      <c r="H3" s="142"/>
+      <c r="I3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="172"/>
-      <c r="K3" s="143" t="s">
+      <c r="J3" s="160"/>
+      <c r="K3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="172"/>
-      <c r="N3" s="156" t="s">
+      <c r="L3" s="160"/>
+      <c r="N3" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="157"/>
-      <c r="P3" s="156" t="s">
+      <c r="O3" s="164"/>
+      <c r="P3" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="Q3" s="157"/>
-      <c r="R3" s="156" t="s">
+      <c r="Q3" s="164"/>
+      <c r="R3" s="163" t="s">
         <v>38</v>
       </c>
-      <c r="S3" s="157"/>
+      <c r="S3" s="164"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1">
       <c r="A4" s="76"/>
@@ -3242,10 +3288,10 @@
       <c r="J4" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="K4" s="77" t="s">
+      <c r="K4" s="179" t="s">
         <v>68</v>
       </c>
-      <c r="L4" s="105" t="s">
+      <c r="L4" s="180" t="s">
         <v>69</v>
       </c>
       <c r="N4" s="114" t="s">
@@ -3268,23 +3314,23 @@
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="139" t="b">
+      <c r="A5" s="137" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="77" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="106">
-        <v>0.89873000000000003</v>
+        <v>0.98873100000000003</v>
       </c>
       <c r="D5" s="107">
-        <v>0.10127</v>
+        <v>1.1269E-2</v>
       </c>
       <c r="E5" s="108">
-        <v>0.95723800000000003</v>
+        <v>0.99079799999999996</v>
       </c>
       <c r="F5" s="107">
-        <v>4.2762000000000001E-2</v>
+        <v>9.2020000000000001E-3</v>
       </c>
       <c r="G5" s="108">
         <v>0.93352000000000002</v>
@@ -3293,16 +3339,16 @@
         <v>6.6479999999999997E-2</v>
       </c>
       <c r="I5" s="106">
-        <v>0.93342199999999997</v>
-      </c>
-      <c r="J5" s="107">
-        <v>6.6577999999999998E-2</v>
+        <v>0.99473500000000004</v>
+      </c>
+      <c r="J5" s="177">
+        <v>5.2649999999999997E-3</v>
       </c>
       <c r="K5" s="106">
-        <v>0.93342199999999997</v>
+        <v>0.989371</v>
       </c>
       <c r="L5" s="107">
-        <v>6.6577999999999998E-2</v>
+        <v>1.0629E-2</v>
       </c>
       <c r="N5" s="116">
         <v>0.93558699999999995</v>
@@ -3320,21 +3366,21 @@
       <c r="S5" s="117"/>
     </row>
     <row r="6" spans="1:19" ht="15" thickBot="1">
-      <c r="A6" s="140"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="78" t="s">
         <v>69</v>
       </c>
       <c r="C6" s="109">
-        <v>2.6848E-2</v>
+        <v>2.2088E-2</v>
       </c>
       <c r="D6" s="110">
-        <v>0.97315200000000002</v>
+        <v>0.977912</v>
       </c>
       <c r="E6" s="111">
-        <v>6.6102999999999995E-2</v>
+        <v>2.5028999999999999E-2</v>
       </c>
       <c r="F6" s="110">
-        <v>0.93389699999999998</v>
+        <v>0.97497100000000003</v>
       </c>
       <c r="G6" s="111">
         <v>0.173815</v>
@@ -3343,16 +3389,16 @@
         <v>0.82618499999999995</v>
       </c>
       <c r="I6" s="109">
-        <v>0.17402899999999999</v>
-      </c>
-      <c r="J6" s="110">
-        <v>0.82597100000000001</v>
+        <v>2.7328999999999999E-2</v>
+      </c>
+      <c r="J6" s="178">
+        <v>0.97267099999999995</v>
       </c>
       <c r="K6" s="109">
-        <v>0.17402899999999999</v>
+        <v>2.2568999999999999E-2</v>
       </c>
       <c r="L6" s="110">
-        <v>0.82597100000000001</v>
+        <v>0.97743100000000005</v>
       </c>
       <c r="N6" s="118">
         <v>0.16606099999999999</v>
@@ -3410,245 +3456,164 @@
         <v>65</v>
       </c>
       <c r="B9" s="94"/>
-      <c r="C9" s="175">
-        <v>0.97315200000000002</v>
-      </c>
-      <c r="D9" s="176"/>
-      <c r="E9" s="175">
-        <v>0.93389699999999998</v>
-      </c>
-      <c r="F9" s="176"/>
-      <c r="G9" s="148">
+      <c r="C9" s="150">
+        <v>0.977912</v>
+      </c>
+      <c r="D9" s="151"/>
+      <c r="E9" s="150">
+        <v>0.97497100000000003</v>
+      </c>
+      <c r="F9" s="151"/>
+      <c r="G9" s="152">
         <v>0.82618499999999995</v>
       </c>
-      <c r="H9" s="149"/>
-      <c r="I9" s="148">
+      <c r="H9" s="153"/>
+      <c r="I9" s="152">
+        <v>0.97267099999999995</v>
+      </c>
+      <c r="J9" s="153"/>
+      <c r="K9" s="152">
+        <v>0.97743100000000005</v>
+      </c>
+      <c r="L9" s="153"/>
+      <c r="N9" s="169">
+        <v>0.83393899999999999</v>
+      </c>
+      <c r="O9" s="170"/>
+      <c r="P9" s="165">
         <v>0.82597100000000001</v>
       </c>
-      <c r="J9" s="149"/>
-      <c r="K9" s="148">
-        <v>0.82597100000000001</v>
-      </c>
-      <c r="L9" s="149"/>
-      <c r="N9" s="164">
-        <v>0.83393899999999999</v>
-      </c>
-      <c r="O9" s="165"/>
-      <c r="P9" s="158">
-        <v>0.82597100000000001</v>
-      </c>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="158"/>
-      <c r="S9" s="159"/>
+      <c r="Q9" s="166"/>
+      <c r="R9" s="165"/>
+      <c r="S9" s="166"/>
     </row>
     <row r="10" spans="1:19" ht="15" thickBot="1">
       <c r="A10" s="93" t="s">
         <v>66</v>
       </c>
       <c r="B10" s="89"/>
-      <c r="C10" s="177">
-        <v>0.10127</v>
-      </c>
-      <c r="D10" s="178"/>
-      <c r="E10" s="177">
-        <v>4.2762000000000001E-2</v>
-      </c>
-      <c r="F10" s="178"/>
-      <c r="G10" s="150">
+      <c r="C10" s="154">
+        <v>1.1269E-2</v>
+      </c>
+      <c r="D10" s="155"/>
+      <c r="E10" s="154">
+        <v>9.2020000000000001E-3</v>
+      </c>
+      <c r="F10" s="155"/>
+      <c r="G10" s="156">
         <v>6.6479999999999997E-2</v>
       </c>
-      <c r="H10" s="151"/>
-      <c r="I10" s="150">
+      <c r="H10" s="157"/>
+      <c r="I10" s="156">
+        <v>5.2649999999999997E-3</v>
+      </c>
+      <c r="J10" s="157"/>
+      <c r="K10" s="156">
+        <v>1.0629E-2</v>
+      </c>
+      <c r="L10" s="157"/>
+      <c r="N10" s="171">
+        <v>6.4412999999999998E-2</v>
+      </c>
+      <c r="O10" s="172"/>
+      <c r="P10" s="167">
         <v>6.6577999999999998E-2</v>
       </c>
-      <c r="J10" s="151"/>
-      <c r="K10" s="150">
-        <v>6.6577999999999998E-2</v>
-      </c>
-      <c r="L10" s="151"/>
-      <c r="N10" s="166">
-        <v>6.4412999999999998E-2</v>
-      </c>
-      <c r="O10" s="167"/>
-      <c r="P10" s="160">
-        <v>6.6577999999999998E-2</v>
-      </c>
-      <c r="Q10" s="161"/>
-      <c r="R10" s="160"/>
-      <c r="S10" s="161"/>
+      <c r="Q10" s="168"/>
+      <c r="R10" s="167"/>
+      <c r="S10" s="168"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="N11" s="121"/>
-      <c r="O11" s="121"/>
-      <c r="P11" s="121"/>
-      <c r="Q11" s="121"/>
-      <c r="R11" s="121"/>
-      <c r="S11" s="121"/>
-    </row>
-    <row r="12" spans="1:19" ht="15" thickBot="1">
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103"/>
-      <c r="G12" s="103"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="103"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="104"/>
-      <c r="N12" s="121"/>
-      <c r="O12" s="121"/>
-      <c r="P12" s="121"/>
-      <c r="Q12" s="122"/>
-      <c r="R12" s="121"/>
-      <c r="S12" s="122"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1">
-      <c r="A13" s="100" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" s="101"/>
-      <c r="C13" s="173"/>
-      <c r="D13" s="174"/>
-      <c r="E13" s="173"/>
-      <c r="F13" s="174"/>
-      <c r="G13" s="152"/>
-      <c r="H13" s="153"/>
-      <c r="I13" s="152"/>
-      <c r="J13" s="153"/>
-      <c r="K13" s="152"/>
-      <c r="L13" s="153"/>
-      <c r="N13" s="168"/>
-      <c r="O13" s="169"/>
-      <c r="P13" s="162"/>
-      <c r="Q13" s="163"/>
-      <c r="R13" s="162"/>
-      <c r="S13" s="163"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="112"/>
+      <c r="L11" s="112"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="112"/>
+      <c r="L12" s="112"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
+      <c r="L13" s="112"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="82"/>
-      <c r="N14" s="113"/>
-      <c r="O14" s="113"/>
-      <c r="P14" s="113"/>
-      <c r="Q14" s="113"/>
-      <c r="R14" s="113"/>
-      <c r="S14" s="113"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="C15" s="112">
-        <v>0.89873000000000003</v>
-      </c>
-      <c r="D15" s="112">
-        <v>0.10127</v>
-      </c>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112"/>
+      <c r="K14" s="112"/>
+      <c r="L14" s="112"/>
+    </row>
+    <row r="15" spans="1:19" ht="15" thickBot="1">
+      <c r="C15" s="112"/>
+      <c r="D15" s="112"/>
       <c r="E15" s="112"/>
       <c r="F15" s="112"/>
       <c r="G15" s="112"/>
       <c r="H15" s="112"/>
-      <c r="I15" s="112">
-        <v>0.93342199999999997</v>
-      </c>
-      <c r="J15" s="112">
-        <v>6.6577999999999998E-2</v>
-      </c>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
       <c r="K15" s="112"/>
       <c r="L15" s="112"/>
-      <c r="N15" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="112">
-        <v>2.6848E-2</v>
-      </c>
-      <c r="D16" s="112">
-        <v>0.97315200000000002</v>
-      </c>
-      <c r="E16" s="112"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="112"/>
-      <c r="H16" s="112"/>
-      <c r="I16" s="112">
-        <v>0.17402899999999999</v>
-      </c>
-      <c r="J16" s="112">
-        <v>0.82597100000000001</v>
-      </c>
-      <c r="K16" s="112"/>
-      <c r="L16" s="112"/>
-    </row>
-    <row r="17" spans="3:12">
-      <c r="C17" s="112"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="112"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="112"/>
-      <c r="H17" s="112"/>
-      <c r="I17" s="112"/>
-      <c r="J17" s="112"/>
-      <c r="K17" s="112"/>
-      <c r="L17" s="112"/>
-    </row>
-    <row r="18" spans="3:12">
-      <c r="C18" s="112">
-        <v>0.97315200000000002</v>
-      </c>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="112">
-        <v>0.82597100000000001</v>
-      </c>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-    </row>
-    <row r="19" spans="3:12">
-      <c r="C19" s="112">
-        <v>0.10127</v>
-      </c>
-      <c r="D19" s="112"/>
-      <c r="E19" s="112"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="112"/>
-      <c r="H19" s="112"/>
-      <c r="I19" s="112">
-        <v>6.6577999999999998E-2</v>
-      </c>
-      <c r="J19" s="112"/>
-      <c r="K19" s="112"/>
-      <c r="L19" s="112"/>
-    </row>
-    <row r="20" spans="3:12">
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="112"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="112"/>
-      <c r="H20" s="112"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="112"/>
-      <c r="K20" s="112"/>
-      <c r="L20" s="112"/>
+      <c r="M16" s="106"/>
+      <c r="N16" s="107"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="I13:J13"/>
+  <mergeCells count="33">
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="R9:S9"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
@@ -3657,35 +3622,6 @@
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="R9:S9"/>
-    <mergeCell ref="R10:S10"/>
-    <mergeCell ref="R13:S13"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P10:Q10"/>
-    <mergeCell ref="P13:Q13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3706,43 +3642,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1">
-      <c r="C1" s="170" t="s">
+      <c r="C1" s="158" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="171"/>
-      <c r="E1" s="170" t="s">
+      <c r="D1" s="159"/>
+      <c r="E1" s="158" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="171"/>
-      <c r="G1" s="170" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="171"/>
-      <c r="I1" s="170" t="s">
+      <c r="F1" s="159"/>
+      <c r="G1" s="158" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="159"/>
+      <c r="I1" s="158" t="s">
         <v>73</v>
       </c>
-      <c r="J1" s="171"/>
+      <c r="J1" s="159"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1"/>
     <row r="3" spans="1:10" ht="15" thickBot="1">
       <c r="A3" s="76"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="141" t="s">
+      <c r="D3" s="140"/>
+      <c r="E3" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="142"/>
-      <c r="G3" s="143" t="s">
+      <c r="F3" s="140"/>
+      <c r="G3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="172"/>
-      <c r="I3" s="143" t="s">
+      <c r="H3" s="160"/>
+      <c r="I3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="172"/>
+      <c r="J3" s="160"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1">
       <c r="A4" s="76"/>
@@ -3773,7 +3709,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="139" t="b">
+      <c r="A5" s="137" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="77" t="s">
@@ -3805,7 +3741,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1">
-      <c r="A6" s="140"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="78" t="s">
         <v>69</v>
       </c>
@@ -3855,48 +3791,48 @@
       <c r="J8" s="112"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="175" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="175">
+      <c r="B9" s="176"/>
+      <c r="C9" s="150">
         <v>0.97315200000000002</v>
       </c>
-      <c r="D9" s="176"/>
-      <c r="E9" s="175">
+      <c r="D9" s="151"/>
+      <c r="E9" s="150">
         <v>0.93389699999999998</v>
       </c>
-      <c r="F9" s="176"/>
-      <c r="G9" s="148">
+      <c r="F9" s="151"/>
+      <c r="G9" s="152">
         <v>0.82597100000000001</v>
       </c>
-      <c r="H9" s="149"/>
-      <c r="I9" s="148">
+      <c r="H9" s="153"/>
+      <c r="I9" s="152">
         <v>0.82597100000000001</v>
       </c>
-      <c r="J9" s="149"/>
+      <c r="J9" s="153"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1">
-      <c r="A10" s="179" t="s">
+      <c r="A10" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="180"/>
-      <c r="C10" s="177">
+      <c r="B10" s="174"/>
+      <c r="C10" s="154">
         <v>0.10127</v>
       </c>
-      <c r="D10" s="178"/>
-      <c r="E10" s="177">
+      <c r="D10" s="155"/>
+      <c r="E10" s="154">
         <v>4.2762000000000001E-2</v>
       </c>
-      <c r="F10" s="178"/>
-      <c r="G10" s="150">
+      <c r="F10" s="155"/>
+      <c r="G10" s="156">
         <v>6.6577999999999998E-2</v>
       </c>
-      <c r="H10" s="151"/>
-      <c r="I10" s="150">
+      <c r="H10" s="157"/>
+      <c r="I10" s="156">
         <v>6.6577999999999998E-2</v>
       </c>
-      <c r="J10" s="151"/>
+      <c r="J10" s="157"/>
     </row>
     <row r="11" spans="1:10">
       <c r="C11" s="103"/>
@@ -3921,22 +3857,25 @@
     <row r="13" spans="1:10" ht="15" thickBot="1">
       <c r="A13" s="100"/>
       <c r="B13" s="101"/>
-      <c r="C13" s="173"/>
-      <c r="D13" s="174"/>
-      <c r="E13" s="173"/>
-      <c r="F13" s="174"/>
-      <c r="G13" s="152"/>
-      <c r="H13" s="153"/>
-      <c r="I13" s="152"/>
-      <c r="J13" s="153"/>
+      <c r="C13" s="146"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="146"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="G3:H3"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="I13:J13"/>
@@ -3947,14 +3886,11 @@
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3965,7 +3901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200A8B2E-17D5-4F5A-B051-63EF40240809}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:J10"/>
     </sheetView>
   </sheetViews>
@@ -3975,43 +3911,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1">
-      <c r="C1" s="170" t="s">
+      <c r="C1" s="158" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="171"/>
-      <c r="E1" s="170" t="s">
+      <c r="D1" s="159"/>
+      <c r="E1" s="158" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="171"/>
-      <c r="G1" s="170" t="s">
+      <c r="F1" s="159"/>
+      <c r="G1" s="158" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="171"/>
-      <c r="I1" s="170" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="171"/>
+      <c r="H1" s="159"/>
+      <c r="I1" s="158" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="159"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1"/>
     <row r="3" spans="1:10" ht="15" thickBot="1">
       <c r="A3" s="76"/>
       <c r="B3" s="76"/>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="D3" s="142"/>
-      <c r="E3" s="141" t="s">
+      <c r="D3" s="140"/>
+      <c r="E3" s="139" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="142"/>
-      <c r="G3" s="143" t="s">
+      <c r="F3" s="140"/>
+      <c r="G3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="172"/>
-      <c r="I3" s="143" t="s">
+      <c r="H3" s="160"/>
+      <c r="I3" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="172"/>
+      <c r="J3" s="160"/>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1">
       <c r="A4" s="76"/>
@@ -4042,7 +3978,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="139" t="b">
+      <c r="A5" s="137" t="b">
         <v>1</v>
       </c>
       <c r="B5" s="77" t="s">
@@ -4070,7 +4006,7 @@
       <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1">
-      <c r="A6" s="140"/>
+      <c r="A6" s="138"/>
       <c r="B6" s="78" t="s">
         <v>69</v>
       </c>
@@ -4116,44 +4052,44 @@
       <c r="J8" s="112"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="181" t="s">
+      <c r="A9" s="175" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="182"/>
-      <c r="C9" s="175">
+      <c r="B9" s="176"/>
+      <c r="C9" s="150">
         <v>0.87282099999999996</v>
       </c>
-      <c r="D9" s="176"/>
-      <c r="E9" s="175">
+      <c r="D9" s="151"/>
+      <c r="E9" s="150">
         <v>0.78762399999999999</v>
       </c>
-      <c r="F9" s="176"/>
-      <c r="G9" s="148">
+      <c r="F9" s="151"/>
+      <c r="G9" s="152">
         <v>0.71194800000000003</v>
       </c>
-      <c r="H9" s="149"/>
-      <c r="I9" s="148"/>
-      <c r="J9" s="149"/>
+      <c r="H9" s="153"/>
+      <c r="I9" s="152"/>
+      <c r="J9" s="153"/>
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1">
-      <c r="A10" s="179" t="s">
+      <c r="A10" s="173" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="180"/>
-      <c r="C10" s="177">
+      <c r="B10" s="174"/>
+      <c r="C10" s="154">
         <v>0.104862</v>
       </c>
-      <c r="D10" s="178"/>
-      <c r="E10" s="177">
+      <c r="D10" s="155"/>
+      <c r="E10" s="154">
         <v>7.7206999999999998E-2</v>
       </c>
-      <c r="F10" s="178"/>
-      <c r="G10" s="150">
+      <c r="F10" s="155"/>
+      <c r="G10" s="156">
         <v>0.11637599999999999</v>
       </c>
-      <c r="H10" s="151"/>
-      <c r="I10" s="150"/>
-      <c r="J10" s="151"/>
+      <c r="H10" s="157"/>
+      <c r="I10" s="156"/>
+      <c r="J10" s="157"/>
     </row>
     <row r="11" spans="1:10">
       <c r="C11" s="103"/>
@@ -4178,17 +4114,25 @@
     <row r="13" spans="1:10" ht="15" thickBot="1">
       <c r="A13" s="100"/>
       <c r="B13" s="101"/>
-      <c r="C13" s="173"/>
-      <c r="D13" s="174"/>
-      <c r="E13" s="173"/>
-      <c r="F13" s="174"/>
-      <c r="G13" s="152"/>
-      <c r="H13" s="153"/>
-      <c r="I13" s="152"/>
-      <c r="J13" s="153"/>
+      <c r="C13" s="146"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="146"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="148"/>
+      <c r="J13" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="G13:H13"/>
@@ -4204,14 +4148,6 @@
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4234,10 +4170,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="128" t="s">
+      <c r="G1" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="129"/>
+      <c r="H1" s="127"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2"/>
@@ -4469,10 +4405,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -5212,10 +5148,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -5947,10 +5883,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -6460,10 +6396,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" s="5" t="s">
         <v>10</v>
       </c>
@@ -6771,11 +6707,11 @@
       <c r="D13" s="4">
         <v>1.51753</v>
       </c>
-      <c r="F13" s="125"/>
-      <c r="G13" s="126"/>
-      <c r="H13" s="126"/>
-      <c r="I13" s="126"/>
-      <c r="J13" s="127"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="124"/>
+      <c r="J13" s="125"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="3">
@@ -7245,10 +7181,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -7555,13 +7491,13 @@
       <c r="D14" s="4">
         <v>1.988488</v>
       </c>
-      <c r="E14" s="125" t="s">
+      <c r="E14" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="127"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="125"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3">
@@ -8020,10 +7956,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -8767,10 +8703,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -9077,13 +9013,13 @@
       <c r="D14" s="4">
         <v>1.988488</v>
       </c>
-      <c r="E14" s="125" t="s">
+      <c r="E14" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="127"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="125"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3">
@@ -9543,10 +9479,10 @@
         <v>0</v>
       </c>
       <c r="E1" s="6"/>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="121" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="124"/>
+      <c r="G1" s="122"/>
       <c r="I1" t="s">
         <v>10</v>
       </c>
@@ -9857,13 +9793,13 @@
       <c r="D14" s="4">
         <v>1.988488</v>
       </c>
-      <c r="E14" s="125" t="s">
+      <c r="E14" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="127"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="125"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="3">
@@ -10766,10 +10702,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="128" t="s">
+      <c r="G1" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="129"/>
+      <c r="H1" s="127"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2"/>
@@ -11004,10 +10940,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="128" t="s">
+      <c r="G1" s="126" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="129"/>
+      <c r="H1" s="127"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="2"/>
@@ -11246,10 +11182,10 @@
   <sheetData>
     <row r="2" spans="3:6">
       <c r="C2" s="46"/>
-      <c r="D2" s="130" t="s">
+      <c r="D2" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="130"/>
+      <c r="E2" s="128"/>
       <c r="F2" s="47"/>
     </row>
     <row r="3" spans="3:6">

</xml_diff>